<commit_message>
docs(day08): link pairwise test cases to related requirements in RTM
</commit_message>
<xml_diff>
--- a/docs/RTM_vo.xlsx
+++ b/docs/RTM_vo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Tracks\Software Testing\QA-20Days-Portfolio\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1575FE65-CD7C-4FDF-BB36-B1AFE322EFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6461DF8-4024-4848-995A-C354EB077763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1695" yWindow="105" windowWidth="18465" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
   <si>
     <t>R-01</t>
   </si>
@@ -187,6 +187,36 @@
   </si>
   <si>
     <t>If the guest user clicks on the wishlist, the should be redirected to the login page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-PW01  </t>
+  </si>
+  <si>
+    <t>TC-PW02</t>
+  </si>
+  <si>
+    <t>TC-PW03</t>
+  </si>
+  <si>
+    <t>TC-PW04</t>
+  </si>
+  <si>
+    <t>TC-PW05</t>
+  </si>
+  <si>
+    <t>TC-PW06</t>
+  </si>
+  <si>
+    <t>TC-PW07</t>
+  </si>
+  <si>
+    <t>TC-PW08</t>
+  </si>
+  <si>
+    <t>TC-PW09</t>
+  </si>
+  <si>
+    <t>TC-PW10</t>
   </si>
 </sst>
 </file>
@@ -275,6 +305,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -287,9 +320,8 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:AD15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -594,180 +626,220 @@
     <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:30" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="7">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8">
         <v>45695</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="Q5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="S5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="T5" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="X5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z5" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD5" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-    </row>
-    <row r="7" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+    </row>
+    <row r="7" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C7" s="1"/>
@@ -776,24 +848,31 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="V7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -803,61 +882,63 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="U9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="4" t="s">
         <v>41</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="4" t="s">
         <v>43</v>
       </c>
       <c r="P13" s="1" t="s">
@@ -867,27 +948,47 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="4" t="s">
         <v>44</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="4" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="36">
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="AA5:AA6"/>
+    <mergeCell ref="AB5:AB6"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="AD5:AD6"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
     <mergeCell ref="S5:S6"/>
     <mergeCell ref="T5:T6"/>
     <mergeCell ref="A1:XFD1"/>
@@ -904,16 +1005,6 @@
     <mergeCell ref="Q5:Q6"/>
     <mergeCell ref="R5:R6"/>
     <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>